<commit_message>
No. 53 Maximum Subarray
</commit_message>
<xml_diff>
--- a/leetcode-tracker.xlsx
+++ b/leetcode-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rudra\Desktop\java-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033CE519-D2FE-476D-AA95-2E73C39D8924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211A533B-FBD6-4CB7-8843-72489E7A9D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Rudy's Leetcode Problem Solving Archives</t>
   </si>
@@ -43,13 +43,22 @@
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+  </si>
+  <si>
+    <t>Guided</t>
+  </si>
+  <si>
+    <t>Self</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +82,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,15 +122,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -403,7 +421,7 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -423,30 +441,46 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="C5" s="3"/>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{1309475C-C6A3-4B4F-9FB4-1669951B10BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>